<commit_message>
Caught missing data bug for COPR EH0, EH40, EH80
Will continue to update affected outputs tomorrow, but all code is working. Think about limits for stacked bars.
</commit_message>
<xml_diff>
--- a/3_Analysis/table6_COPR_at_004080.xlsx
+++ b/3_Analysis/table6_COPR_at_004080.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boterolab1/Box Sync/CB_VF_Shared/Wet_Lab/Projects/FS/FS_Analysis/3_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2133EC28-7FAC-CA48-9234-92EA8905A176}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B28CC0-A83F-5C4C-8D95-753C96434548}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{2E521CEB-226C-0649-817F-20FAD0BA4998}"/>
+    <workbookView xWindow="34060" yWindow="3640" windowWidth="25600" windowHeight="15540" xr2:uid="{2E521CEB-226C-0649-817F-20FAD0BA4998}"/>
   </bookViews>
   <sheets>
     <sheet name="table6_COPR_at_004080_inc_raw" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="13">
   <si>
     <t>n_tot</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>EH0</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>011</t>
   </si>
 </sst>
 </file>
@@ -98,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,9 +429,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A286B3A0-087B-A247-B41F-68F89F8768C7}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -444,8 +462,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -470,7 +488,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
@@ -496,7 +514,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -522,8 +540,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -548,7 +566,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>110</v>
       </c>
       <c r="B6">
@@ -574,7 +592,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>101</v>
       </c>
       <c r="B7">
@@ -600,8 +618,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -626,7 +644,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>111</v>
       </c>
       <c r="B9">
@@ -652,7 +670,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10">
@@ -678,7 +696,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">
@@ -712,9 +730,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547D3394-7A89-F64B-A1F2-BB19FBA2CF39}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -740,8 +763,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>3.1E-2</v>
@@ -766,7 +789,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
@@ -792,7 +815,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -818,8 +841,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -844,7 +867,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>110</v>
       </c>
       <c r="B6">
@@ -870,7 +893,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>101</v>
       </c>
       <c r="B7">
@@ -896,8 +919,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -922,7 +945,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>111</v>
       </c>
       <c r="B9">
@@ -948,7 +971,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10">
@@ -974,7 +997,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">
@@ -1008,9 +1031,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A4A8E8-2033-CD4A-8E4E-39F9DDBE2B55}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -1036,8 +1064,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -1062,7 +1090,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
@@ -1088,7 +1116,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -1114,8 +1142,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1140,7 +1168,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>110</v>
       </c>
       <c r="B6">
@@ -1166,7 +1194,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>101</v>
       </c>
       <c r="B7">
@@ -1192,8 +1220,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1218,7 +1246,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>111</v>
       </c>
       <c r="B9">
@@ -1244,7 +1272,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10">
@@ -1270,7 +1298,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">
@@ -1304,9 +1332,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24426A4D-A418-3F4A-8F88-84B844E0EB53}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -1332,8 +1365,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1358,7 +1391,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
@@ -1384,7 +1417,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -1410,8 +1443,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1436,7 +1469,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>110</v>
       </c>
       <c r="B6">
@@ -1462,7 +1495,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>101</v>
       </c>
       <c r="B7">
@@ -1488,8 +1521,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1514,7 +1547,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>111</v>
       </c>
       <c r="B9">
@@ -1540,7 +1573,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10">
@@ -1566,7 +1599,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">
@@ -1600,9 +1633,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAB66EF-707D-CE46-BD75-A53CC1CE7459}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -1628,8 +1666,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0.312</v>
@@ -1654,7 +1692,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
@@ -1680,7 +1718,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -1706,8 +1744,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1732,7 +1770,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>110</v>
       </c>
       <c r="B6">
@@ -1758,7 +1796,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>101</v>
       </c>
       <c r="B7">
@@ -1784,8 +1822,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1810,7 +1848,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>111</v>
       </c>
       <c r="B9">
@@ -1836,7 +1874,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10">
@@ -1862,7 +1900,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">
@@ -1896,9 +1934,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F434C4-B12B-484C-A4F7-E207C95AB471}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -1924,8 +1967,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1950,7 +1993,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
@@ -1976,7 +2019,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -2002,8 +2045,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2028,7 +2071,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>110</v>
       </c>
       <c r="B6">
@@ -2054,7 +2097,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>101</v>
       </c>
       <c r="B7">
@@ -2080,8 +2123,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2106,7 +2149,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>111</v>
       </c>
       <c r="B9">
@@ -2132,7 +2175,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10">
@@ -2158,7 +2201,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">

</xml_diff>